<commit_message>
Reuseablity added in quick quote
</commit_message>
<xml_diff>
--- a/binaries/CGFiles/AddProductsTemplate.xlsx
+++ b/binaries/CGFiles/AddProductsTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cymax-my.sharepoint.com/personal/samta_k_cymax_com/Documents/Desktop/work/CG-post-prod/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\binaries\CGFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_889FC8D4B261CBA174E4716F11F4E2256F5BB455" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{936EBDA8-7221-4F2C-BD15-AB66D1E1C869}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7727F580-452A-45CD-B879-B7E5D1CCB57E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -9617,19 +9617,19 @@
     <t>https://media.cymaxstores.com/Images/4991/1813684-1-L.jpg</t>
   </si>
   <si>
-    <t>Test05-06</t>
-  </si>
-  <si>
-    <t>Test05-07</t>
-  </si>
-  <si>
-    <t>Test05-08</t>
-  </si>
-  <si>
-    <t>Test05-09</t>
-  </si>
-  <si>
-    <t>Test05-10</t>
+    <t>Test056-06</t>
+  </si>
+  <si>
+    <t>Test056-07</t>
+  </si>
+  <si>
+    <t>Test056-08</t>
+  </si>
+  <si>
+    <t>Test056-09</t>
+  </si>
+  <si>
+    <t>Test056-10</t>
   </si>
 </sst>
 </file>
@@ -10242,25 +10242,25 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" customWidth="1"/>
-    <col min="2" max="2" width="53.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="38.08984375" customWidth="1"/>
-    <col min="6" max="6" width="91.453125" customWidth="1"/>
-    <col min="7" max="7" width="68.453125" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" customWidth="1"/>
-    <col min="9" max="9" width="14.08984375" customWidth="1"/>
-    <col min="10" max="10" width="17.08984375" customWidth="1"/>
-    <col min="11" max="11" width="35.36328125" customWidth="1"/>
-    <col min="12" max="12" width="84.453125" customWidth="1"/>
-    <col min="13" max="13" width="9.36328125" customWidth="1"/>
-    <col min="14" max="14" width="63.36328125" customWidth="1"/>
-    <col min="15" max="15" width="9.36328125" customWidth="1"/>
-    <col min="16" max="16" width="18.90625" customWidth="1"/>
-    <col min="17" max="17" width="9.08984375" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" customWidth="1"/>
+    <col min="6" max="6" width="91.42578125" customWidth="1"/>
+    <col min="7" max="7" width="68.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" customWidth="1"/>
+    <col min="12" max="12" width="84.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="63.42578125" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -24953,77 +24953,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BR70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A7"/>
+      <selection pane="bottomLeft" activeCell="AZ4" sqref="AZ4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.90625" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
-    <col min="6" max="6" width="46.36328125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" customWidth="1"/>
     <col min="7" max="7" width="50" customWidth="1"/>
-    <col min="8" max="8" width="29.6328125" customWidth="1"/>
-    <col min="9" max="9" width="15.08984375" customWidth="1"/>
-    <col min="10" max="10" width="30.08984375" customWidth="1"/>
-    <col min="11" max="14" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" customWidth="1"/>
+    <col min="11" max="14" width="12.42578125" customWidth="1"/>
     <col min="15" max="15" width="23" customWidth="1"/>
-    <col min="16" max="16" width="25.453125" customWidth="1"/>
-    <col min="17" max="17" width="20.6328125" customWidth="1"/>
-    <col min="18" max="18" width="24.36328125" customWidth="1"/>
-    <col min="19" max="19" width="20.6328125" customWidth="1"/>
-    <col min="20" max="20" width="22.453125" customWidth="1"/>
-    <col min="21" max="21" width="20.6328125" customWidth="1"/>
-    <col min="22" max="22" width="22.453125" customWidth="1"/>
-    <col min="23" max="23" width="20.6328125" customWidth="1"/>
-    <col min="24" max="24" width="22.453125" customWidth="1"/>
-    <col min="25" max="25" width="16.36328125" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" customWidth="1"/>
+    <col min="18" max="18" width="24.42578125" customWidth="1"/>
+    <col min="19" max="19" width="20.5703125" customWidth="1"/>
+    <col min="20" max="20" width="22.42578125" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" customWidth="1"/>
+    <col min="22" max="22" width="22.42578125" customWidth="1"/>
+    <col min="23" max="23" width="20.5703125" customWidth="1"/>
+    <col min="24" max="24" width="22.42578125" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" customWidth="1"/>
     <col min="26" max="26" width="29" customWidth="1"/>
-    <col min="27" max="27" width="21.54296875" customWidth="1"/>
-    <col min="28" max="28" width="9.36328125" customWidth="1"/>
-    <col min="29" max="29" width="12.6328125" customWidth="1"/>
-    <col min="30" max="30" width="12.453125" customWidth="1"/>
-    <col min="31" max="31" width="17.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.5703125" customWidth="1"/>
+    <col min="28" max="28" width="9.42578125" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" customWidth="1"/>
+    <col min="31" max="31" width="17.5703125" style="36" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="18" customWidth="1"/>
-    <col min="33" max="33" width="14.453125" customWidth="1"/>
-    <col min="34" max="34" width="9.36328125" customWidth="1"/>
-    <col min="35" max="35" width="12.90625" customWidth="1"/>
-    <col min="36" max="36" width="14.453125" customWidth="1"/>
-    <col min="37" max="37" width="9.54296875" customWidth="1"/>
-    <col min="38" max="38" width="16.90625" customWidth="1"/>
-    <col min="39" max="39" width="17.90625" customWidth="1"/>
-    <col min="40" max="40" width="20.36328125" customWidth="1"/>
-    <col min="41" max="41" width="16.90625" customWidth="1"/>
-    <col min="42" max="42" width="20.90625" customWidth="1"/>
-    <col min="43" max="43" width="23.453125" customWidth="1"/>
-    <col min="44" max="44" width="20.90625" customWidth="1"/>
-    <col min="45" max="45" width="18.453125" customWidth="1"/>
+    <col min="33" max="33" width="14.42578125" customWidth="1"/>
+    <col min="34" max="34" width="9.42578125" customWidth="1"/>
+    <col min="35" max="35" width="12.85546875" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" customWidth="1"/>
+    <col min="37" max="37" width="9.5703125" customWidth="1"/>
+    <col min="38" max="38" width="16.85546875" customWidth="1"/>
+    <col min="39" max="39" width="17.85546875" customWidth="1"/>
+    <col min="40" max="40" width="20.42578125" customWidth="1"/>
+    <col min="41" max="41" width="16.85546875" customWidth="1"/>
+    <col min="42" max="42" width="20.85546875" customWidth="1"/>
+    <col min="43" max="43" width="23.42578125" customWidth="1"/>
+    <col min="44" max="44" width="20.85546875" customWidth="1"/>
+    <col min="45" max="45" width="18.42578125" customWidth="1"/>
     <col min="46" max="46" width="14" customWidth="1"/>
-    <col min="47" max="47" width="16.90625" customWidth="1"/>
-    <col min="48" max="48" width="12.36328125" customWidth="1"/>
-    <col min="49" max="49" width="17.08984375" customWidth="1"/>
-    <col min="50" max="51" width="16.6328125" customWidth="1"/>
-    <col min="52" max="52" width="17.6328125" customWidth="1"/>
-    <col min="53" max="53" width="19.08984375" customWidth="1"/>
-    <col min="54" max="55" width="18.6328125" customWidth="1"/>
-    <col min="56" max="56" width="19.6328125" customWidth="1"/>
-    <col min="57" max="57" width="21.08984375" customWidth="1"/>
-    <col min="58" max="58" width="17.54296875" customWidth="1"/>
-    <col min="59" max="59" width="16.90625" customWidth="1"/>
-    <col min="60" max="60" width="19.08984375" customWidth="1"/>
-    <col min="61" max="62" width="18.6328125" customWidth="1"/>
-    <col min="63" max="63" width="19.6328125" customWidth="1"/>
-    <col min="64" max="64" width="21.08984375" customWidth="1"/>
-    <col min="65" max="65" width="17.54296875" customWidth="1"/>
-    <col min="66" max="66" width="16.90625" customWidth="1"/>
-    <col min="67" max="67" width="51.81640625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="33.90625" customWidth="1"/>
-    <col min="69" max="70" width="14.36328125" customWidth="1"/>
-    <col min="71" max="71" width="9.08984375" customWidth="1"/>
+    <col min="47" max="47" width="16.85546875" customWidth="1"/>
+    <col min="48" max="48" width="12.42578125" customWidth="1"/>
+    <col min="49" max="49" width="17.140625" customWidth="1"/>
+    <col min="50" max="51" width="16.5703125" customWidth="1"/>
+    <col min="52" max="52" width="17.5703125" customWidth="1"/>
+    <col min="53" max="53" width="19.140625" customWidth="1"/>
+    <col min="54" max="55" width="18.5703125" customWidth="1"/>
+    <col min="56" max="56" width="19.5703125" customWidth="1"/>
+    <col min="57" max="57" width="21.140625" customWidth="1"/>
+    <col min="58" max="58" width="17.5703125" customWidth="1"/>
+    <col min="59" max="59" width="16.85546875" customWidth="1"/>
+    <col min="60" max="60" width="19.140625" customWidth="1"/>
+    <col min="61" max="62" width="18.5703125" customWidth="1"/>
+    <col min="63" max="63" width="19.5703125" customWidth="1"/>
+    <col min="64" max="64" width="21.140625" customWidth="1"/>
+    <col min="65" max="65" width="17.5703125" customWidth="1"/>
+    <col min="66" max="66" width="16.85546875" customWidth="1"/>
+    <col min="67" max="67" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="33.85546875" customWidth="1"/>
+    <col min="69" max="70" width="14.42578125" customWidth="1"/>
+    <col min="71" max="71" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70">

</xml_diff>